<commit_message>
updated annex and cbo transformation
</commit_message>
<xml_diff>
--- a/models/US_OOS/data/US_info.xlsx
+++ b/models/US_OOS/data/US_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Desktop/inflation_mixed_freq/models/US_no_core_rt/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Desktop/inflation_mixed_freq/models/US_OOS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0FB512-575F-7047-A748-4F0225EB346B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB0D193-7476-5049-8114-95ED177E3DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Prof Forecasters: Median: 1-Year-Ahead CPI Inflation Expectation (%)</t>
   </si>
@@ -104,9 +104,6 @@
     <t>TRANSF</t>
   </si>
   <si>
-    <t>TRANSF_ANNEX</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -123,6 +120,12 @@
   </si>
   <si>
     <t>Compute SPF expectation in levels, starting from the growth rates (wrt the variable specified in TRANSF_ANNEX)</t>
+  </si>
+  <si>
+    <t>TRANSF_ARG1</t>
+  </si>
+  <si>
+    <t>TRANSF_ARG2</t>
   </si>
 </sst>
 </file>
@@ -570,20 +573,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="88.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="13.33203125" style="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.83203125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="13.33203125" style="1" customWidth="1"/>
+    <col min="7" max="1025" width="8.83203125" style="1" customWidth="1"/>
     <col min="1026" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -597,10 +598,13 @@
         <v>21</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>28</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -614,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -628,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -642,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -656,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -670,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
@@ -687,7 +691,7 @@
         <v>7824.2470000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -700,11 +704,11 @@
       <c r="D8" s="1">
         <v>3</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
@@ -732,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FDC31C-0E1C-1D4D-9192-FF775FADE936}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -746,7 +750,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -754,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -762,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -770,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -778,7 +782,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -786,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>